<commit_message>
edited with team comments
</commit_message>
<xml_diff>
--- a/Grants.xlsx
+++ b/Grants.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Grants to Campus for Programs (in thousands of dollars)</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Other(Gift and adminstrative fees, Interest earnings granted, Cost recovery fees on investment goods)</t>
   </si>
 </sst>
 </file>
@@ -387,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,6 +561,27 @@
       <c r="E10">
         <f>SUM(E3:E9)</f>
         <v>68307</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <f>SUM(B7:B9)</f>
+        <v>3908</v>
+      </c>
+      <c r="C11">
+        <f>SUM(C7:C9)</f>
+        <v>6944</v>
+      </c>
+      <c r="D11">
+        <f>SUM(D7:D9)</f>
+        <v>7009</v>
+      </c>
+      <c r="E11">
+        <f>SUM(E7:E9)</f>
+        <v>8070</v>
       </c>
     </row>
   </sheetData>

</xml_diff>